<commit_message>
DB supports type of field for array of strings
</commit_message>
<xml_diff>
--- a/data/news/posts.xlsx
+++ b/data/news/posts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">main_image</t>
+  </si>
+  <si>
     <t xml:space="preserve">images</t>
   </si>
   <si>
@@ -52,6 +55,26 @@
     <t xml:space="preserve">Title 1</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">data/news/images/n-01.jpg
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">data/news/images/n-02.jpg</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">2021-08-02</t>
   </si>
   <si>
@@ -61,6 +84,9 @@
     <t xml:space="preserve">Title 2</t>
   </si>
   <si>
+    <t xml:space="preserve">data/news/images/n-02.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">author1</t>
   </si>
   <si>
@@ -83,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">Title 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data/news/images/n-03.jpg</t>
   </si>
 </sst>
 </file>
@@ -93,7 +122,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -114,6 +143,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,6 +207,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -192,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,9 +242,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1007" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="37.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1008" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,22 +267,28 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,16 +296,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,16 +319,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,16 +336,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>